<commit_message>
Mengubah index pasien menjadi id pasien
</commit_message>
<xml_diff>
--- a/Perhitungan.xlsx
+++ b/Perhitungan.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/95499214ec9b6c66/Documents/TUGAS ONGOING/SMS 4/PRAK SCPK/ProjectAkhir/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/95499214ec9b6c66/Documents/TUGAS ONGOING/SMS 4/PRAK SCPK/ProjectAkhir/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{7A107D86-1ADB-4DB3-ADFA-C3E920490094}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{399C6231-7ED5-4A36-8E36-02DB99C2F7C9}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="8_{7A107D86-1ADB-4DB3-ADFA-C3E920490094}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7EAB1982-1AFC-4D29-A30A-2D38E9515ABE}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -380,30 +380,39 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -411,15 +420,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -703,8 +703,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="D5:Q59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D48" workbookViewId="0">
-      <selection activeCell="M63" sqref="M63"/>
+    <sheetView tabSelected="1" topLeftCell="D40" workbookViewId="0">
+      <selection activeCell="O64" sqref="O64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -770,10 +770,10 @@
       <c r="O7" s="4"/>
     </row>
     <row r="8" spans="4:15">
-      <c r="D8" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="E8" s="14"/>
+      <c r="D8" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="E8" s="20"/>
       <c r="F8" s="3" t="s">
         <v>2</v>
       </c>
@@ -951,10 +951,10 @@
       <c r="F17" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G17" s="14" t="s">
+      <c r="G17" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="H17" s="14"/>
+      <c r="H17" s="20"/>
     </row>
     <row r="18" spans="4:9">
       <c r="D18" s="3" t="s">
@@ -967,11 +967,11 @@
         <f t="shared" ref="F18:F30" si="0">(E18/$E$31)</f>
         <v>8.8235294117647065E-2</v>
       </c>
-      <c r="G18" s="18">
+      <c r="G18" s="21">
         <f>(F18*G9)</f>
         <v>8.8235294117647065E-2</v>
       </c>
-      <c r="H18" s="18"/>
+      <c r="H18" s="21"/>
       <c r="I18" t="s">
         <v>4</v>
       </c>
@@ -987,11 +987,11 @@
         <f t="shared" si="0"/>
         <v>2.9411764705882353E-2</v>
       </c>
-      <c r="G19" s="18">
+      <c r="G19" s="21">
         <f>(F19*G10)</f>
         <v>-2.9411764705882353E-2</v>
       </c>
-      <c r="H19" s="18"/>
+      <c r="H19" s="21"/>
       <c r="I19" t="s">
         <v>6</v>
       </c>
@@ -1007,11 +1007,11 @@
         <f t="shared" si="0"/>
         <v>8.8235294117647065E-2</v>
       </c>
-      <c r="G20" s="18">
+      <c r="G20" s="21">
         <f>(F20*G11)</f>
         <v>8.8235294117647065E-2</v>
       </c>
-      <c r="H20" s="18"/>
+      <c r="H20" s="21"/>
       <c r="I20" t="s">
         <v>7</v>
       </c>
@@ -1027,11 +1027,11 @@
         <f t="shared" si="0"/>
         <v>0.11764705882352941</v>
       </c>
-      <c r="G21" s="18">
+      <c r="G21" s="21">
         <f>(F21*G12)</f>
         <v>0.11764705882352941</v>
       </c>
-      <c r="H21" s="18"/>
+      <c r="H21" s="21"/>
       <c r="I21" t="s">
         <v>8</v>
       </c>
@@ -1047,11 +1047,11 @@
         <f t="shared" si="0"/>
         <v>5.8823529411764705E-2</v>
       </c>
-      <c r="G22" s="18">
+      <c r="G22" s="21">
         <f>(F22*G12)</f>
         <v>5.8823529411764705E-2</v>
       </c>
-      <c r="H22" s="18"/>
+      <c r="H22" s="21"/>
       <c r="I22" t="s">
         <v>10</v>
       </c>
@@ -1067,11 +1067,11 @@
         <f t="shared" si="0"/>
         <v>0.14705882352941177</v>
       </c>
-      <c r="G23" s="19">
+      <c r="G23" s="22">
         <f>F23*1</f>
         <v>0.14705882352941177</v>
       </c>
-      <c r="H23" s="20"/>
+      <c r="H23" s="23"/>
       <c r="I23" t="s">
         <v>33</v>
       </c>
@@ -1087,11 +1087,11 @@
         <f t="shared" si="0"/>
         <v>5.8823529411764705E-2</v>
       </c>
-      <c r="G24" s="19">
+      <c r="G24" s="22">
         <f t="shared" ref="G24:G30" si="1">F24*1</f>
         <v>5.8823529411764705E-2</v>
       </c>
-      <c r="H24" s="20"/>
+      <c r="H24" s="23"/>
       <c r="I24" t="s">
         <v>34</v>
       </c>
@@ -1107,11 +1107,11 @@
         <f t="shared" si="0"/>
         <v>8.8235294117647065E-2</v>
       </c>
-      <c r="G25" s="19">
+      <c r="G25" s="22">
         <f t="shared" si="1"/>
         <v>8.8235294117647065E-2</v>
       </c>
-      <c r="H25" s="20"/>
+      <c r="H25" s="23"/>
       <c r="I25" t="s">
         <v>35</v>
       </c>
@@ -1127,11 +1127,11 @@
         <f t="shared" si="0"/>
         <v>5.8823529411764705E-2</v>
       </c>
-      <c r="G26" s="19">
+      <c r="G26" s="22">
         <f t="shared" si="1"/>
         <v>5.8823529411764705E-2</v>
       </c>
-      <c r="H26" s="20"/>
+      <c r="H26" s="23"/>
       <c r="I26" t="s">
         <v>36</v>
       </c>
@@ -1147,11 +1147,11 @@
         <f t="shared" si="0"/>
         <v>8.8235294117647065E-2</v>
       </c>
-      <c r="G27" s="19">
+      <c r="G27" s="22">
         <f t="shared" si="1"/>
         <v>8.8235294117647065E-2</v>
       </c>
-      <c r="H27" s="20"/>
+      <c r="H27" s="23"/>
       <c r="I27" t="s">
         <v>37</v>
       </c>
@@ -1167,11 +1167,11 @@
         <f t="shared" si="0"/>
         <v>2.9411764705882353E-2</v>
       </c>
-      <c r="G28" s="19">
+      <c r="G28" s="22">
         <f>F28*1</f>
         <v>2.9411764705882353E-2</v>
       </c>
-      <c r="H28" s="20"/>
+      <c r="H28" s="23"/>
       <c r="I28" t="s">
         <v>38</v>
       </c>
@@ -1187,11 +1187,11 @@
         <f t="shared" si="0"/>
         <v>5.8823529411764705E-2</v>
       </c>
-      <c r="G29" s="19">
+      <c r="G29" s="22">
         <f t="shared" si="1"/>
         <v>5.8823529411764705E-2</v>
       </c>
-      <c r="H29" s="20"/>
+      <c r="H29" s="23"/>
       <c r="I29" t="s">
         <v>39</v>
       </c>
@@ -1207,11 +1207,11 @@
         <f t="shared" si="0"/>
         <v>8.8235294117647065E-2</v>
       </c>
-      <c r="G30" s="19">
+      <c r="G30" s="22">
         <f t="shared" si="1"/>
         <v>8.8235294117647065E-2</v>
       </c>
-      <c r="H30" s="20"/>
+      <c r="H30" s="23"/>
       <c r="I30" t="s">
         <v>40</v>
       </c>
@@ -1235,19 +1235,19 @@
       </c>
     </row>
     <row r="35" spans="4:17">
-      <c r="D35" s="14" t="s">
+      <c r="D35" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="E35" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="F35" s="14"/>
-      <c r="G35" s="14"/>
-      <c r="H35" s="14"/>
-      <c r="I35" s="14"/>
+      <c r="E35" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="F35" s="20"/>
+      <c r="G35" s="20"/>
+      <c r="H35" s="20"/>
+      <c r="I35" s="20"/>
     </row>
     <row r="36" spans="4:17">
-      <c r="D36" s="14"/>
+      <c r="D36" s="20"/>
       <c r="E36" s="2" t="s">
         <v>4</v>
       </c>
@@ -1471,19 +1471,19 @@
       <c r="E43" s="1"/>
     </row>
     <row r="44" spans="4:17">
-      <c r="D44" s="14" t="s">
+      <c r="D44" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="E44" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="F44" s="14"/>
-      <c r="G44" s="14"/>
-      <c r="H44" s="14"/>
-      <c r="I44" s="14"/>
+      <c r="E44" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="F44" s="20"/>
+      <c r="G44" s="20"/>
+      <c r="H44" s="20"/>
+      <c r="I44" s="20"/>
     </row>
     <row r="45" spans="4:17">
-      <c r="D45" s="14"/>
+      <c r="D45" s="20"/>
       <c r="E45" s="2" t="s">
         <v>4</v>
       </c>
@@ -1757,55 +1757,55 @@
       <c r="E50" s="1"/>
     </row>
     <row r="52" spans="4:17">
-      <c r="D52" s="14" t="s">
+      <c r="D52" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="E52" s="14"/>
-      <c r="F52" s="14"/>
-      <c r="G52" s="14"/>
-      <c r="H52" s="14"/>
-      <c r="I52" s="14"/>
-      <c r="J52" s="10" t="s">
+      <c r="E52" s="20"/>
+      <c r="F52" s="20"/>
+      <c r="G52" s="20"/>
+      <c r="H52" s="20"/>
+      <c r="I52" s="20"/>
+      <c r="J52" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="K52" s="10"/>
-      <c r="L52" s="11" t="s">
+      <c r="K52" s="16"/>
+      <c r="L52" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="O52" s="10" t="s">
+      <c r="O52" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="P52" s="10"/>
-      <c r="Q52" s="11" t="s">
+      <c r="P52" s="16"/>
+      <c r="Q52" s="10" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="53" spans="4:17">
-      <c r="D53" s="10"/>
-      <c r="E53" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="F53" s="10"/>
-      <c r="G53" s="10"/>
-      <c r="H53" s="10"/>
-      <c r="I53" s="10"/>
-      <c r="J53" s="14" t="s">
+      <c r="D53" s="16"/>
+      <c r="E53" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="F53" s="16"/>
+      <c r="G53" s="16"/>
+      <c r="H53" s="16"/>
+      <c r="I53" s="16"/>
+      <c r="J53" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="K53" s="14" t="s">
+      <c r="K53" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="L53" s="12"/>
-      <c r="O53" s="14" t="s">
+      <c r="L53" s="11"/>
+      <c r="O53" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="P53" s="14" t="s">
+      <c r="P53" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="Q53" s="12"/>
+      <c r="Q53" s="11"/>
     </row>
     <row r="54" spans="4:17">
-      <c r="D54" s="10"/>
+      <c r="D54" s="16"/>
       <c r="E54" s="2" t="s">
         <v>4</v>
       </c>
@@ -1821,12 +1821,12 @@
       <c r="I54" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="J54" s="14"/>
-      <c r="K54" s="14"/>
-      <c r="L54" s="13"/>
-      <c r="O54" s="14"/>
-      <c r="P54" s="14"/>
-      <c r="Q54" s="13"/>
+      <c r="J54" s="20"/>
+      <c r="K54" s="20"/>
+      <c r="L54" s="12"/>
+      <c r="O54" s="20"/>
+      <c r="P54" s="20"/>
+      <c r="Q54" s="12"/>
     </row>
     <row r="55" spans="4:17">
       <c r="D55" s="2" t="s">
@@ -1860,9 +1860,12 @@
         <f>(J55/$J$59)</f>
         <v>0.34656164615910373</v>
       </c>
-      <c r="L55" s="15">
+      <c r="L55" s="13">
         <f>MAX(K55:K57)</f>
         <v>0.38136965126321654</v>
+      </c>
+      <c r="N55">
+        <v>1</v>
       </c>
       <c r="O55" s="6">
         <f>E46*F46*G46*H46*I46*J46*K46*L46*M46*N46*O46*P46*Q46</f>
@@ -1872,7 +1875,7 @@
         <f>O55/O59</f>
         <v>0.19332695223357704</v>
       </c>
-      <c r="Q55" s="15">
+      <c r="Q55" s="13">
         <f>MAX(P55:P58)</f>
         <v>0.35361164794916272</v>
       </c>
@@ -1909,7 +1912,10 @@
         <f>(J56/$J$59)</f>
         <v>0.27206870257767968</v>
       </c>
-      <c r="L56" s="16"/>
+      <c r="L56" s="14"/>
+      <c r="N56">
+        <v>2</v>
+      </c>
       <c r="O56" s="6">
         <f t="shared" ref="O56:O58" si="12">E47*F47*G47*H47*I47*J47*K47*L47*M47*N47*O47*P47*Q47</f>
         <v>3.1210304074475959</v>
@@ -1918,7 +1924,7 @@
         <f>O56/O59</f>
         <v>0.15663436044771598</v>
       </c>
-      <c r="Q56" s="16"/>
+      <c r="Q56" s="14"/>
     </row>
     <row r="57" spans="4:17">
       <c r="D57" s="2" t="s">
@@ -1952,7 +1958,10 @@
         <f>(J57/$J$59)</f>
         <v>0.38136965126321654</v>
       </c>
-      <c r="L57" s="16"/>
+      <c r="L57" s="14"/>
+      <c r="N57">
+        <v>3</v>
+      </c>
       <c r="O57" s="6">
         <f t="shared" si="12"/>
         <v>5.9064805501014463</v>
@@ -1961,7 +1970,7 @@
         <f>O57/O59</f>
         <v>0.2964270393695444</v>
       </c>
-      <c r="Q57" s="16"/>
+      <c r="Q57" s="14"/>
     </row>
     <row r="58" spans="4:17">
       <c r="D58" s="4"/>
@@ -1972,7 +1981,10 @@
       <c r="I58" s="4"/>
       <c r="J58" s="4"/>
       <c r="K58" s="4"/>
-      <c r="L58" s="17"/>
+      <c r="L58" s="15"/>
+      <c r="N58">
+        <v>4</v>
+      </c>
       <c r="O58" s="6">
         <f t="shared" si="12"/>
         <v>7.0459170166904723</v>
@@ -1981,17 +1993,17 @@
         <f>O58/O59</f>
         <v>0.35361164794916272</v>
       </c>
-      <c r="Q58" s="17"/>
+      <c r="Q58" s="15"/>
     </row>
     <row r="59" spans="4:17">
-      <c r="D59" s="21" t="s">
+      <c r="D59" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="E59" s="22"/>
-      <c r="F59" s="22"/>
-      <c r="G59" s="22"/>
-      <c r="H59" s="22"/>
-      <c r="I59" s="23"/>
+      <c r="E59" s="18"/>
+      <c r="F59" s="18"/>
+      <c r="G59" s="18"/>
+      <c r="H59" s="18"/>
+      <c r="I59" s="19"/>
       <c r="J59" s="6">
         <f>SUM(J55:J57)</f>
         <v>6.0629456108620143</v>
@@ -2007,13 +2019,16 @@
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="L52:L54"/>
-    <mergeCell ref="L55:L58"/>
-    <mergeCell ref="E53:I53"/>
-    <mergeCell ref="D59:I59"/>
-    <mergeCell ref="D35:D36"/>
-    <mergeCell ref="D53:D54"/>
-    <mergeCell ref="J53:J54"/>
+    <mergeCell ref="O52:P52"/>
+    <mergeCell ref="Q52:Q54"/>
+    <mergeCell ref="O53:O54"/>
+    <mergeCell ref="P53:P54"/>
+    <mergeCell ref="Q55:Q58"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="G20:H20"/>
     <mergeCell ref="G21:H21"/>
     <mergeCell ref="G30:H30"/>
     <mergeCell ref="E35:I35"/>
@@ -2026,20 +2041,17 @@
     <mergeCell ref="G29:H29"/>
     <mergeCell ref="D44:D45"/>
     <mergeCell ref="E44:I44"/>
-    <mergeCell ref="K53:K54"/>
     <mergeCell ref="G22:H22"/>
     <mergeCell ref="G23:H23"/>
     <mergeCell ref="G24:H24"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="O52:P52"/>
-    <mergeCell ref="Q52:Q54"/>
-    <mergeCell ref="O53:O54"/>
-    <mergeCell ref="P53:P54"/>
-    <mergeCell ref="Q55:Q58"/>
+    <mergeCell ref="L52:L54"/>
+    <mergeCell ref="L55:L58"/>
+    <mergeCell ref="E53:I53"/>
+    <mergeCell ref="D59:I59"/>
+    <mergeCell ref="D35:D36"/>
+    <mergeCell ref="D53:D54"/>
+    <mergeCell ref="J53:J54"/>
+    <mergeCell ref="K53:K54"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>